<commit_message>
Feat : Make HUD Base
- Add HUDWidget in PlayerController
- Link StatData with HUD.
</commit_message>
<xml_diff>
--- a/GameData/SLCharacterStatTable.xlsx
+++ b/GameData/SLCharacterStatTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongchan\Documents\Unreal Projects\SekiroLike\GameData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongchan\Documents\Unreal Projects\SekiroLike\UnrealSoloProject\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C10962-2E37-45B2-8ECC-C5B0E9136194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FDC8F3-3205-48AC-BED3-CFF3856F4F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5145" yWindow="23880" windowWidth="29040" windowHeight="15720" xr2:uid="{14535CBB-5647-4022-885E-3A0FC95BEC4B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{14535CBB-5647-4022-885E-3A0FC95BEC4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="2" r:id="rId1"/>
@@ -445,7 +445,7 @@
   <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>

</xml_diff>